<commit_message>
made difficulty estimation faster and more accurate
</commit_message>
<xml_diff>
--- a/documentation/results.xlsx
+++ b/documentation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micha\Desktop\FinalYearProject2022\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5064422-C4F1-494B-BCEE-414B036F3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC8E29B-F0F2-4CA7-9A9E-AA7C4098A7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trivial Level" sheetId="1" r:id="rId1"/>
@@ -533,6 +533,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -559,10 +560,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -571,7 +569,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Non Trivial Level</a:t>
+              <a:t>Non Trivial Level </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -591,10 +589,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -870,10 +865,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -902,10 +894,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -939,10 +928,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -989,10 +975,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1021,10 +1004,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1053,10 +1033,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1095,10 +1072,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1140,7 +1114,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1150,6 +1128,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2307,6 +2286,88 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.23667</cdr:x>
+      <cdr:y>0.66667</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.43667</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10D658CD-9435-45E5-BB22-CB7F97793DE7}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1082040" y="2506980"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00333</cdr:x>
+      <cdr:y>0.01667</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.17</cdr:x>
+      <cdr:y>0.09486</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="7" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB62E30-FCB3-46F9-BBB3-CA3B7A91707A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="15241" y="45720"/>
+          <a:ext cx="761999" cy="214488"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2345,6 +2406,51 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00839</cdr:x>
+      <cdr:y>0.01654</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.12457</cdr:x>
+      <cdr:y>0.08106</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="5" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5719B2F-9155-4E20-917D-ECE88F922ED6}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="50800" y="50800"/>
+          <a:ext cx="703847" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2612,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
@@ -2664,7 +2770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD17E2-A92E-4F35-90A1-3AFB42924659}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>